<commit_message>
Add DriverName when export report
</commit_message>
<xml_diff>
--- a/WebAPI/Transportation/wwwroot/ReportTemplate/Bangke.xlsx
+++ b/WebAPI/Transportation/wwwroot/ReportTemplate/Bangke.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>BẢNG KÊ VẬN CHUYỂN THÁNG 11</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>CHI PHÍ CTY ( 5%)</t>
+  </si>
+  <si>
+    <t>TÀI XẾ</t>
+  </si>
+  <si>
+    <t>PHỤ XE</t>
   </si>
 </sst>
 </file>
@@ -311,7 +317,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -420,6 +426,9 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -10939,7 +10948,7 @@
   <dimension ref="A1:K1643"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75"/>
@@ -10952,7 +10961,7 @@
     <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="21" customWidth="1"/>
     <col min="8" max="8" width="24.125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.375" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="6" customWidth="1"/>
     <col min="11" max="11" width="15.875" style="6" customWidth="1"/>
     <col min="12" max="12" width="29" style="6" customWidth="1"/>
@@ -11207,6 +11216,8 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="12" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -11233,8 +11244,12 @@
       <c r="H4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="I4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" s="13" customFormat="1">
@@ -11248,6 +11263,8 @@
       <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="3"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
     </row>
     <row r="6" spans="1:11" s="13" customFormat="1">
       <c r="A6" s="14" t="s">
@@ -11260,6 +11277,8 @@
       <c r="F6" s="17"/>
       <c r="G6" s="18"/>
       <c r="H6" s="9"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:11" s="13" customFormat="1">
       <c r="A7" s="14" t="s">
@@ -11272,6 +11291,8 @@
       <c r="F7" s="20"/>
       <c r="G7" s="18"/>
       <c r="H7" s="9"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:11" s="13" customFormat="1">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
Add new UI for add transportation
</commit_message>
<xml_diff>
--- a/WebAPI/Transportation/wwwroot/ReportTemplate/Bangke.xlsx
+++ b/WebAPI/Transportation/wwwroot/ReportTemplate/Bangke.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BẢNG TỔNG HỢP" sheetId="1" r:id="rId1"/>
     <sheet name="sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="BẢNG LƯƠNG" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'BẢNG TỔNG HỢP'!$A$1:$H$16</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>BẢNG KÊ VẬN CHUYỂN THÁNG 11</t>
   </si>
@@ -105,10 +106,7 @@
     <t>CHI PHÍ CTY ( 5%)</t>
   </si>
   <si>
-    <t>TÀI XẾ</t>
-  </si>
-  <si>
-    <t>PHỤ XE</t>
+    <t>BẢNG LƯƠNG TÀI XẾ &amp; PHỤ XE</t>
   </si>
 </sst>
 </file>
@@ -120,7 +118,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +201,32 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -317,7 +341,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -412,6 +436,19 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,8 +464,14 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -950,28 +993,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:11" s="8" customFormat="1">
       <c r="A3" s="3" t="s">
@@ -1070,11 +1113,11 @@
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
     </row>
     <row r="10" spans="1:11" s="13" customFormat="1">
       <c r="A10" s="1"/>
@@ -1082,11 +1125,11 @@
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:11" s="13" customFormat="1">
       <c r="A11" s="1"/>
@@ -1139,11 +1182,11 @@
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" s="13" customFormat="1">
       <c r="A17" s="1"/>
@@ -10947,8 +10990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1643"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75"/>
@@ -11180,28 +11223,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:11" s="8" customFormat="1">
       <c r="A3" s="3" t="s">
@@ -11216,8 +11261,8 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:11" s="12" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -11244,12 +11289,8 @@
       <c r="H4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" s="13" customFormat="1">
@@ -11263,8 +11304,8 @@
       <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:11" s="13" customFormat="1">
       <c r="A6" s="14" t="s">
@@ -11277,8 +11318,8 @@
       <c r="F6" s="17"/>
       <c r="G6" s="18"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:11" s="13" customFormat="1">
       <c r="A7" s="14" t="s">
@@ -11291,8 +11332,8 @@
       <c r="F7" s="20"/>
       <c r="G7" s="18"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" s="13" customFormat="1">
       <c r="A8" s="1"/>
@@ -21172,4 +21213,59 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="6.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" customHeight="1">
+      <c r="A1" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>